<commit_message>
Update template with PA, SAC; rename scoresheet
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="0" windowWidth="21620" windowHeight="14140"/>
+    <workbookView xWindow="540" yWindow="120" windowWidth="21620" windowHeight="14140"/>
   </bookViews>
   <sheets>
     <sheet name="MLS scorecard" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'MLS scorecard'!$A$1:$K$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'MLS scorecard'!$A$1:$L$20</definedName>
   </definedNames>
   <calcPr calcId="114210" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>vs.</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Final score:</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>SAC</t>
   </si>
 </sst>
 </file>
@@ -186,8 +192,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -228,22 +242,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -260,20 +259,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -291,6 +305,10 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -308,6 +326,10 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -637,299 +659,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J20"/>
+  <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" style="8" customWidth="1"/>
-    <col min="2" max="10" width="10" style="8" customWidth="1"/>
-    <col min="11" max="11" width="4.33203125" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="8"/>
+    <col min="1" max="1" width="25.33203125" style="3" customWidth="1"/>
+    <col min="2" max="12" width="10" style="3" customWidth="1"/>
+    <col min="13" max="13" width="4.33203125" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A3" s="12" t="s">
+      <c r="H2" s="15"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" ht="21.75" customHeight="1">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" ht="21.75" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="1:10" ht="21.75" customHeight="1"/>
-    <row r="6" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A6" s="15" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" ht="21.75" customHeight="1"/>
+    <row r="6" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="D6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="H6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="I6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="J6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="K6" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A7" s="16">
+      <c r="L6" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A7" s="10">
         <v>1</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A8" s="17">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A8" s="11">
         <v>2</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A9" s="17">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A9" s="11">
         <v>3</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A10" s="17">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A10" s="11">
         <v>4</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A11" s="17">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A11" s="11">
         <v>5</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A12" s="17">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A12" s="11">
         <v>6</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A13" s="17">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A13" s="11">
         <v>7</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A14" s="17">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A14" s="11">
         <v>8</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A15" s="17">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A15" s="11">
         <v>9</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-    </row>
-    <row r="16" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A16" s="17">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A16" s="11">
         <v>10</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-    </row>
-    <row r="17" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A17" s="17">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A17" s="11">
         <v>11</v>
       </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-    </row>
-    <row r="18" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A18" s="17">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A18" s="11">
         <v>12</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-    </row>
-    <row r="19" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A19" s="17">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A19" s="11">
         <v>13</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-    </row>
-    <row r="20" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A20" s="17">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" ht="21.75" customHeight="1">
+      <c r="A20" s="11">
         <v>14</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="H2:J2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
-  <pageSetup scale="95" orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294"/>
+  <pageSetup scale="87" orientation="landscape" horizontalDpi="4294967294" verticalDpi="4294967294"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>